<commit_message>
Atualização do sistema de registros com melhorias em gráficos e orçamentos
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Registros" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Gráficos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Orçamentos" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,8 +56,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -717,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -783,104 +784,48 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-10-15</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>10</v>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>JOSE GENILSOS MARTINS SOARES</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Outro</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>EXTERNO</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>12:30:00</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-10-17</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>11</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>NETANIS DOS SANTOS</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Marcenaria Estrutural</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CDS</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>14:27:00</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>15:00:00</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ODS</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>15:50</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>registro</t>
         </is>
@@ -897,39 +842,158 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Área/Projeto</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Horas Trabalhadas</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Horas Orçadas</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Horas Restantes</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Percentual (%)</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural - CDS - 12</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural - CDS - 15</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural - FÁBRICA - 12</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural - ODS - 12</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural - TDS - 15</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Marcenaria Móvel - CDS - 12</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Marcenaria Móvel - ODS - 12</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -939,4 +1003,191 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Área</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Projeto</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Número Projeto</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Horas Orçadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Marcenaria Móvel</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ODS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TDS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ODS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FÁBRICA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Marcenaria Móvel</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel file with latest budgets and charts
- Updated Orçamentos sheet with current budget data
- Updated Gráficos sheet with charts for budgeted projects
- Charts now show worked vs budgeted hours for projects with budgets
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -159,11 +159,6 @@
         <ser>
           <idx val="0"/>
           <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Gráficos'!B1</f>
-            </strRef>
-          </tx>
           <spPr>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -171,23 +166,18 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$1</f>
+              <f>'Gráficos'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$C$1:$B$1</f>
+              <f>'Gráficos'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
         <ser>
           <idx val="1"/>
           <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Gráficos'!C1</f>
-            </strRef>
-          </tx>
           <spPr>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -195,36 +185,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$1</f>
+              <f>'Gráficos'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$D$1:$C$1</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Gráficos'!D1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Gráficos'!$A$2:$A$1</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Gráficos'!$E$1:$D$1</f>
+              <f>'Gráficos'!$C$2:$C$3</f>
             </numRef>
           </val>
         </ser>
@@ -325,12 +291,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$1</f>
+              <f>'Gráficos'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$E$2:$E$1</f>
+              <f>'Gráficos'!$E$2:$E$3</f>
             </numRef>
           </val>
         </ser>
@@ -344,12 +310,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$1</f>
+              <f>'Gráficos'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$D$2:$D$1</f>
+              <f>'Gráficos'!$D$2:$D$3</f>
             </numRef>
           </val>
         </ser>
@@ -718,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,45 +753,233 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>007</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DENILSON DE SOUZA SANTOS</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Marcenaria Estrutural</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>14:50:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15:50:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>007</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DENILSON DE SOUZA SANTOS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Outro</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FÁBRICA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>14:50:00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>15:50:00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>010</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>JOSE GENILSOS MARTINS SOARES</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ODS</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>15:50</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>16:05</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Outro</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>EXTERNO</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>14:55:00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>JOSE GENILSOS MARTINS SOARES</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Hidráulica</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TOT</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>15:05:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>JOSE GENILSOS MARTINS SOARES</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Piso</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>FÁBRICA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>15:05:00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>15:11:00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>registro</t>
         </is>
@@ -842,7 +996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -899,104 +1053,186 @@
       <c r="D2" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Marcenaria Estrutural - CDS - 15</t>
+          <t>Marcenaria Móvel - ODS - 12</t>
         </is>
       </c>
       <c r="B3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural - FÁBRICA - 12</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>0</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural - ODS - 12</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural - TDS - 15</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Marcenaria Móvel - CDS - 12</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Marcenaria Móvel - ODS - 12</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   <tableParts count="1">
@@ -1011,7 +1247,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1060,11 +1296,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -1084,106 +1320,6 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CDS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TDS</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ODS</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Marcenaria Estrutural</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>FÁBRICA</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Marcenaria Móvel</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CDS</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add file existence checks to /verificar and /registrar routes
- /verificar: Returns error if registros.xlsx is missing
- /registrar: Returns error if registros.xlsx is missing
- Prevents crashes when Excel file is not present
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -166,12 +166,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$3</f>
+              <f>'Gráficos'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$B$2:$B$3</f>
+              <f>'Gráficos'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -185,12 +185,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$3</f>
+              <f>'Gráficos'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$C$2:$C$3</f>
+              <f>'Gráficos'!$C$2:$C$4</f>
             </numRef>
           </val>
         </ser>
@@ -291,12 +291,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$3</f>
+              <f>'Gráficos'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$E$2:$E$3</f>
+              <f>'Gráficos'!$E$2:$E$4</f>
             </numRef>
           </val>
         </ser>
@@ -310,12 +310,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Gráficos'!$A$2:$A$3</f>
+              <f>'Gráficos'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Gráficos'!$D$2:$D$3</f>
+              <f>'Gráficos'!$D$2:$D$4</f>
             </numRef>
           </val>
         </ser>
@@ -684,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -985,6 +985,53 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>JOSE GENILSOS MARTINS SOARES</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Elétrica</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>VDS</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>15:40:00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>16:40:00</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>registro</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -996,7 +1043,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,17 +1088,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marcenaria Estrutural - CDS - 12</t>
+          <t>Hidráulica - LOGISTÍCA - 1</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0</v>
@@ -1060,19 +1107,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Marcenaria Estrutural - CDS - 12</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Marcenaria Móvel - ODS - 12</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C4" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D4" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1200,6 +1266,16 @@
         <color rgb="0000FF00"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="dataBar" priority="14">
@@ -1216,6 +1292,13 @@
         <color rgb="000000FF"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
     <cfRule type="dataBar" priority="15">
@@ -1226,6 +1309,43 @@
       </dataBar>
     </cfRule>
     <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="0000FF00"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="000000FF"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1247,7 +1367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1323,6 +1443,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hidráulica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LOGISTÍCA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>